<commit_message>
added code for experiment 2
</commit_message>
<xml_diff>
--- a/Caroline/Stimuli Experiment 2/stimuliOverview.xlsx
+++ b/Caroline/Stimuli Experiment 2/stimuliOverview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="168">
   <si>
     <t>target</t>
   </si>
@@ -117,15 +117,9 @@
     <t>corn</t>
   </si>
   <si>
-    <t>cucumber</t>
-  </si>
-  <si>
     <t>broccoli</t>
   </si>
   <si>
-    <t>pear</t>
-  </si>
-  <si>
     <t>kiwi</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>bed</t>
   </si>
   <si>
-    <t>lamp</t>
-  </si>
-  <si>
     <t>cupboard</t>
   </si>
   <si>
@@ -150,18 +141,12 @@
     <t>lengthString</t>
   </si>
   <si>
-    <t>cello</t>
-  </si>
-  <si>
     <t>flute</t>
   </si>
   <si>
     <t>saxophone</t>
   </si>
   <si>
-    <t>clarinete</t>
-  </si>
-  <si>
     <t>car</t>
   </si>
   <si>
@@ -171,9 +156,6 @@
     <t>schoolbus</t>
   </si>
   <si>
-    <t>garbagetruck</t>
-  </si>
-  <si>
     <t>tree</t>
   </si>
   <si>
@@ -192,9 +174,6 @@
     <t>sunflower</t>
   </si>
   <si>
-    <t>daffodil</t>
-  </si>
-  <si>
     <t>hut</t>
   </si>
   <si>
@@ -267,9 +246,6 @@
     <t>motorcycle</t>
   </si>
   <si>
-    <t>truck</t>
-  </si>
-  <si>
     <t>cactus</t>
   </si>
   <si>
@@ -291,9 +267,6 @@
     <t>violet</t>
   </si>
   <si>
-    <t>iris</t>
-  </si>
-  <si>
     <t>igloo</t>
   </si>
   <si>
@@ -351,9 +324,6 @@
     <t>firehydrant</t>
   </si>
   <si>
-    <t>binocculars</t>
-  </si>
-  <si>
     <t>garbagecan</t>
   </si>
   <si>
@@ -366,12 +336,6 @@
     <t>sameSSClassDistr2</t>
   </si>
   <si>
-    <t>artifactDistr1</t>
-  </si>
-  <si>
-    <t>artifactDistr2</t>
-  </si>
-  <si>
     <t>gloves</t>
   </si>
   <si>
@@ -390,36 +354,15 @@
     <t>mushroom</t>
   </si>
   <si>
-    <t>bacteriia</t>
-  </si>
-  <si>
-    <t>maple tree</t>
-  </si>
-  <si>
-    <t>herb</t>
-  </si>
-  <si>
-    <t>shrub</t>
-  </si>
-  <si>
-    <t>vine</t>
-  </si>
-  <si>
     <t>grasses</t>
   </si>
   <si>
-    <t>strawberryplant</t>
-  </si>
-  <si>
     <t>cherryTree</t>
   </si>
   <si>
     <t>chive</t>
   </si>
   <si>
-    <t>office</t>
-  </si>
-  <si>
     <t>shop</t>
   </si>
   <si>
@@ -429,18 +372,6 @@
     <t>school</t>
   </si>
   <si>
-    <t>library</t>
-  </si>
-  <si>
-    <t>communityCenter</t>
-  </si>
-  <si>
-    <t>gym</t>
-  </si>
-  <si>
-    <t>bank</t>
-  </si>
-  <si>
     <t>penguin</t>
   </si>
   <si>
@@ -481,6 +412,117 @@
   </si>
   <si>
     <t>palmTree</t>
+  </si>
+  <si>
+    <t>banjo</t>
+  </si>
+  <si>
+    <t>zucchini</t>
+  </si>
+  <si>
+    <t>lime</t>
+  </si>
+  <si>
+    <t>clarinet</t>
+  </si>
+  <si>
+    <t>firetruck</t>
+  </si>
+  <si>
+    <t>cherryBlossom</t>
+  </si>
+  <si>
+    <t>couch</t>
+  </si>
+  <si>
+    <t>garbageTruck</t>
+  </si>
+  <si>
+    <t>hyacinth</t>
+  </si>
+  <si>
+    <t>rubberduck</t>
+  </si>
+  <si>
+    <t>teddybear</t>
+  </si>
+  <si>
+    <t>tire</t>
+  </si>
+  <si>
+    <t>toilet</t>
+  </si>
+  <si>
+    <t>tooth</t>
+  </si>
+  <si>
+    <t>tophat</t>
+  </si>
+  <si>
+    <t>pencil</t>
+  </si>
+  <si>
+    <t>eraser</t>
+  </si>
+  <si>
+    <t>binoculars</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>backpack</t>
+  </si>
+  <si>
+    <t>shirt</t>
+  </si>
+  <si>
+    <t>shoes</t>
+  </si>
+  <si>
+    <t>hamster</t>
+  </si>
+  <si>
+    <t>snake</t>
+  </si>
+  <si>
+    <t>lobster</t>
+  </si>
+  <si>
+    <t>sheep</t>
+  </si>
+  <si>
+    <t>elephant</t>
+  </si>
+  <si>
+    <t>fir</t>
+  </si>
+  <si>
+    <t>rosemary</t>
+  </si>
+  <si>
+    <t>ivy</t>
+  </si>
+  <si>
+    <t>pottedPlant</t>
+  </si>
+  <si>
+    <t>strawberryPlant</t>
+  </si>
+  <si>
+    <t>barber</t>
+  </si>
+  <si>
+    <t>church</t>
+  </si>
+  <si>
+    <t>trainStation</t>
+  </si>
+  <si>
+    <t>airport</t>
+  </si>
+  <si>
+    <t>restaurant</t>
   </si>
 </sst>
 </file>
@@ -889,15 +931,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -908,10 +950,10 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -923,19 +965,13 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="J1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K1" t="s">
-        <v>115</v>
-      </c>
-      <c r="L1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -948,8 +984,11 @@
       <c r="D2">
         <v>3</v>
       </c>
+      <c r="E2">
+        <v>41</v>
+      </c>
       <c r="F2" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -961,10 +1000,10 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -977,23 +1016,26 @@
       <c r="D3">
         <v>3</v>
       </c>
+      <c r="E3">
+        <v>180</v>
+      </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1006,8 +1048,11 @@
       <c r="D4">
         <v>9</v>
       </c>
+      <c r="E4">
+        <v>49</v>
+      </c>
       <c r="F4" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -1019,15 +1064,15 @@
         <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1035,8 +1080,11 @@
       <c r="D5">
         <v>9</v>
       </c>
+      <c r="E5">
+        <v>204</v>
+      </c>
       <c r="F5" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -1048,10 +1096,10 @@
         <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1064,6 +1112,9 @@
       <c r="D6">
         <v>4</v>
       </c>
+      <c r="E6">
+        <v>607</v>
+      </c>
       <c r="F6" t="s">
         <v>19</v>
       </c>
@@ -1071,16 +1122,16 @@
         <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="I6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="J6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1093,6 +1144,9 @@
       <c r="D7">
         <v>4</v>
       </c>
+      <c r="E7">
+        <v>1171</v>
+      </c>
       <c r="F7" t="s">
         <v>19</v>
       </c>
@@ -1100,21 +1154,21 @@
         <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="J7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -1122,6 +1176,9 @@
       <c r="D8">
         <v>8</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
       <c r="F8" t="s">
         <v>19</v>
       </c>
@@ -1129,21 +1186,21 @@
         <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="J8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -1151,6 +1208,9 @@
       <c r="D9">
         <v>8</v>
       </c>
+      <c r="E9">
+        <v>132</v>
+      </c>
       <c r="F9" t="s">
         <v>19</v>
       </c>
@@ -1158,21 +1218,21 @@
         <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="I9" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="J9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -1180,28 +1240,31 @@
       <c r="D10">
         <v>4</v>
       </c>
+      <c r="E10">
+        <v>641</v>
+      </c>
       <c r="F10" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="G10" t="s">
         <v>26</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I10" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="J10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -1209,28 +1272,31 @@
       <c r="D11">
         <v>4</v>
       </c>
+      <c r="E11">
+        <v>189</v>
+      </c>
       <c r="F11" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="G11" t="s">
         <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -1238,28 +1304,31 @@
       <c r="D12">
         <v>9</v>
       </c>
+      <c r="E12">
+        <v>275</v>
+      </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="G12" t="s">
         <v>26</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I12" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="J12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1267,28 +1336,31 @@
       <c r="D13">
         <v>10</v>
       </c>
+      <c r="E13">
+        <v>129</v>
+      </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="G13" t="s">
         <v>26</v>
       </c>
       <c r="H13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="I13" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="J13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -1296,6 +1368,9 @@
       <c r="D14">
         <v>3</v>
       </c>
+      <c r="E14">
+        <v>14695</v>
+      </c>
       <c r="F14" t="s">
         <v>20</v>
       </c>
@@ -1303,24 +1378,30 @@
         <v>27</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>93</v>
+      </c>
+      <c r="J14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>7388</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
@@ -1329,18 +1410,21 @@
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>94</v>
+      </c>
+      <c r="J15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -1348,6 +1432,9 @@
       <c r="D16">
         <v>8</v>
       </c>
+      <c r="E16">
+        <v>1358</v>
+      </c>
       <c r="F16" t="s">
         <v>20</v>
       </c>
@@ -1355,10 +1442,13 @@
         <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I16" t="s">
-        <v>104</v>
+        <v>95</v>
+      </c>
+      <c r="J16" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1366,7 +1456,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -1374,6 +1464,9 @@
       <c r="D17">
         <v>9</v>
       </c>
+      <c r="E17">
+        <v>70</v>
+      </c>
       <c r="F17" t="s">
         <v>20</v>
       </c>
@@ -1381,10 +1474,13 @@
         <v>27</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
       <c r="I17" t="s">
-        <v>105</v>
+        <v>96</v>
+      </c>
+      <c r="J17" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1392,7 +1488,7 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -1400,6 +1496,9 @@
       <c r="D18">
         <v>5</v>
       </c>
+      <c r="E18">
+        <v>186</v>
+      </c>
       <c r="F18" t="s">
         <v>21</v>
       </c>
@@ -1407,10 +1506,13 @@
         <v>27</v>
       </c>
       <c r="H18" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="I18" t="s">
-        <v>106</v>
+        <v>97</v>
+      </c>
+      <c r="J18" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1418,7 +1520,7 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -1426,6 +1528,9 @@
       <c r="D19">
         <v>5</v>
       </c>
+      <c r="E19">
+        <v>381</v>
+      </c>
       <c r="F19" t="s">
         <v>21</v>
       </c>
@@ -1433,10 +1538,13 @@
         <v>27</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I19" t="s">
-        <v>107</v>
+        <v>98</v>
+      </c>
+      <c r="J19" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1444,7 +1552,7 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -1452,6 +1560,9 @@
       <c r="D20">
         <v>9</v>
       </c>
+      <c r="E20">
+        <v>87</v>
+      </c>
       <c r="F20" t="s">
         <v>21</v>
       </c>
@@ -1459,10 +1570,13 @@
         <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I20" t="s">
-        <v>108</v>
+        <v>99</v>
+      </c>
+      <c r="J20" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1470,13 +1584,16 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>240</v>
       </c>
       <c r="F21" t="s">
         <v>21</v>
@@ -1485,10 +1602,13 @@
         <v>27</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I21" t="s">
-        <v>109</v>
+        <v>100</v>
+      </c>
+      <c r="J21" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1496,7 +1616,7 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1504,6 +1624,9 @@
       <c r="D22">
         <v>3</v>
       </c>
+      <c r="E22">
+        <v>26886</v>
+      </c>
       <c r="F22" t="s">
         <v>22</v>
       </c>
@@ -1511,10 +1634,13 @@
         <v>27</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="I22" t="s">
-        <v>110</v>
+        <v>148</v>
+      </c>
+      <c r="J22" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1522,7 +1648,7 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
@@ -1530,6 +1656,9 @@
       <c r="D23">
         <v>4</v>
       </c>
+      <c r="E23">
+        <v>1763</v>
+      </c>
       <c r="F23" t="s">
         <v>22</v>
       </c>
@@ -1537,10 +1666,13 @@
         <v>27</v>
       </c>
       <c r="H23" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="I23" t="s">
-        <v>111</v>
+        <v>101</v>
+      </c>
+      <c r="J23" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1548,7 +1680,7 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -1556,6 +1688,9 @@
       <c r="D24">
         <v>9</v>
       </c>
+      <c r="E24">
+        <v>62</v>
+      </c>
       <c r="F24" t="s">
         <v>22</v>
       </c>
@@ -1563,10 +1698,13 @@
         <v>27</v>
       </c>
       <c r="H24" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I24" t="s">
-        <v>112</v>
+        <v>102</v>
+      </c>
+      <c r="J24" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1574,13 +1712,16 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
       </c>
       <c r="F25" t="s">
         <v>22</v>
@@ -1589,10 +1730,13 @@
         <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="I25" t="s">
-        <v>117</v>
+        <v>105</v>
+      </c>
+      <c r="J25" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1600,7 +1744,7 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
@@ -1608,6 +1752,9 @@
       <c r="D26">
         <v>4</v>
       </c>
+      <c r="E26">
+        <v>6136</v>
+      </c>
       <c r="F26" t="s">
         <v>23</v>
       </c>
@@ -1615,13 +1762,13 @@
         <v>28</v>
       </c>
       <c r="H26" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I26" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="J26" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1629,7 +1776,7 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
@@ -1637,6 +1784,9 @@
       <c r="D27">
         <v>4</v>
       </c>
+      <c r="E27">
+        <v>3717</v>
+      </c>
       <c r="F27" t="s">
         <v>23</v>
       </c>
@@ -1644,13 +1794,13 @@
         <v>28</v>
       </c>
       <c r="H27" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="J27" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1658,7 +1808,7 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -1666,6 +1816,9 @@
       <c r="D28">
         <v>9</v>
       </c>
+      <c r="E28">
+        <v>140</v>
+      </c>
       <c r="F28" t="s">
         <v>23</v>
       </c>
@@ -1673,13 +1826,13 @@
         <v>28</v>
       </c>
       <c r="H28" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I28" t="s">
-        <v>11</v>
+        <v>154</v>
       </c>
       <c r="J28" t="s">
-        <v>13</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1687,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -1695,6 +1848,9 @@
       <c r="D29">
         <v>8</v>
       </c>
+      <c r="E29">
+        <v>35</v>
+      </c>
       <c r="F29" t="s">
         <v>23</v>
       </c>
@@ -1702,13 +1858,13 @@
         <v>28</v>
       </c>
       <c r="H29" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="I29" t="s">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="J29" t="s">
-        <v>14</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1716,7 +1872,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C30" t="b">
         <v>1</v>
@@ -1724,6 +1880,9 @@
       <c r="D30">
         <v>4</v>
       </c>
+      <c r="E30">
+        <v>10639</v>
+      </c>
       <c r="F30" t="s">
         <v>24</v>
       </c>
@@ -1731,13 +1890,13 @@
         <v>23</v>
       </c>
       <c r="H30" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="I30" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="J30" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1745,7 +1904,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C31" t="b">
         <v>1</v>
@@ -1753,6 +1912,9 @@
       <c r="D31">
         <v>5</v>
       </c>
+      <c r="E31">
+        <v>622</v>
+      </c>
       <c r="F31" t="s">
         <v>24</v>
       </c>
@@ -1760,13 +1922,13 @@
         <v>23</v>
       </c>
       <c r="H31" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I31" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="J31" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1774,7 +1936,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -1782,6 +1944,9 @@
       <c r="D32">
         <v>9</v>
       </c>
+      <c r="E32">
+        <v>115</v>
+      </c>
       <c r="F32" t="s">
         <v>24</v>
       </c>
@@ -1789,13 +1954,13 @@
         <v>23</v>
       </c>
       <c r="H32" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="I32" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="J32" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1803,13 +1968,16 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="E33">
+        <v>22</v>
       </c>
       <c r="F33" t="s">
         <v>24</v>
@@ -1818,13 +1986,13 @@
         <v>23</v>
       </c>
       <c r="H33" t="s">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="I33" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="J33" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1832,13 +2000,16 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C34" t="b">
         <v>1</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>22</v>
       </c>
       <c r="F34" t="s">
         <v>25</v>
@@ -1847,13 +2018,13 @@
         <v>29</v>
       </c>
       <c r="H34" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="I34" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="J34" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1861,7 +2032,7 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C35" t="b">
         <v>1</v>
@@ -1869,6 +2040,9 @@
       <c r="D35">
         <v>4</v>
       </c>
+      <c r="E35">
+        <v>1097</v>
+      </c>
       <c r="F35" t="s">
         <v>25</v>
       </c>
@@ -1876,13 +2050,13 @@
         <v>29</v>
       </c>
       <c r="H35" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I35" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="J35" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1890,7 +2064,7 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -1898,6 +2072,9 @@
       <c r="D36">
         <v>9</v>
       </c>
+      <c r="E36">
+        <v>30</v>
+      </c>
       <c r="F36" t="s">
         <v>25</v>
       </c>
@@ -1905,13 +2082,13 @@
         <v>29</v>
       </c>
       <c r="H36" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="I36" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="J36" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1919,7 +2096,7 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -1927,6 +2104,9 @@
       <c r="D37">
         <v>9</v>
       </c>
+      <c r="E37">
+        <v>1233</v>
+      </c>
       <c r="F37" t="s">
         <v>25</v>
       </c>
@@ -1934,13 +2114,13 @@
         <v>29</v>
       </c>
       <c r="H37" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="I37" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="J37" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated experiment norming stuff
</commit_message>
<xml_diff>
--- a/Caroline/Stimuli Experiment 2/stimuliOverview.xlsx
+++ b/Caroline/Stimuli Experiment 2/stimuliOverview.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="17540" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="186">
   <si>
     <t>target</t>
   </si>
@@ -183,9 +183,6 @@
     <t>treehouse</t>
   </si>
   <si>
-    <t>apartment</t>
-  </si>
-  <si>
     <t>BNCfreq</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>cottage</t>
   </si>
   <si>
-    <t>caravan</t>
-  </si>
-  <si>
     <t>castle</t>
   </si>
   <si>
@@ -429,18 +423,12 @@
     <t>firetruck</t>
   </si>
   <si>
-    <t>cherryBlossom</t>
-  </si>
-  <si>
     <t>couch</t>
   </si>
   <si>
     <t>garbageTruck</t>
   </si>
   <si>
-    <t>hyacinth</t>
-  </si>
-  <si>
     <t>rubberduck</t>
   </si>
   <si>
@@ -523,13 +511,79 @@
   </si>
   <si>
     <t>restaurant</t>
+  </si>
+  <si>
+    <t>whole dog</t>
+  </si>
+  <si>
+    <t>cut out ship train</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>get new idandelion</t>
+  </si>
+  <si>
+    <t>trailer</t>
+  </si>
+  <si>
+    <t>get 2 more</t>
+  </si>
+  <si>
+    <t>treehouse?</t>
+  </si>
+  <si>
+    <t>highrise</t>
+  </si>
+  <si>
+    <t>orchid</t>
+  </si>
+  <si>
+    <t>dress</t>
+  </si>
+  <si>
+    <t>pants</t>
+  </si>
+  <si>
+    <t>jeans</t>
+  </si>
+  <si>
+    <t>socks</t>
+  </si>
+  <si>
+    <t>underwear</t>
+  </si>
+  <si>
+    <t>belt</t>
+  </si>
+  <si>
+    <t>bra</t>
+  </si>
+  <si>
+    <t>leggings</t>
+  </si>
+  <si>
+    <t>tank top</t>
+  </si>
+  <si>
+    <t>sweater</t>
+  </si>
+  <si>
+    <t>skirt</t>
+  </si>
+  <si>
+    <t>swimsuit</t>
+  </si>
+  <si>
+    <t>bikini</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -549,6 +603,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -586,8 +647,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -931,15 +993,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -953,7 +1015,7 @@
         <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -965,13 +1027,13 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
@@ -988,7 +1050,7 @@
         <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -1000,10 +1062,10 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1020,7 +1082,7 @@
         <v>180</v>
       </c>
       <c r="F3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -1032,10 +1094,13 @@
         <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>116</v>
+      </c>
+      <c r="M3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1052,7 +1117,7 @@
         <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -1064,10 +1129,13 @@
         <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>117</v>
+      </c>
+      <c r="L4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1084,7 +1152,7 @@
         <v>204</v>
       </c>
       <c r="F5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -1096,10 +1164,10 @@
         <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1122,16 +1190,16 @@
         <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1154,21 +1222,21 @@
         <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -1186,16 +1254,16 @@
         <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1218,21 +1286,21 @@
         <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -1244,22 +1312,22 @@
         <v>641</v>
       </c>
       <c r="F10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G10" t="s">
         <v>26</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1276,22 +1344,22 @@
         <v>189</v>
       </c>
       <c r="F11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G11" t="s">
         <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1308,22 +1376,22 @@
         <v>275</v>
       </c>
       <c r="F12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G12" t="s">
         <v>26</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1340,22 +1408,22 @@
         <v>129</v>
       </c>
       <c r="F13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G13" t="s">
         <v>26</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1378,21 +1446,21 @@
         <v>27</v>
       </c>
       <c r="H14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -1410,16 +1478,16 @@
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J15" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1442,16 +1510,16 @@
         <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1474,21 +1542,21 @@
         <v>27</v>
       </c>
       <c r="H17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -1506,16 +1574,16 @@
         <v>27</v>
       </c>
       <c r="H18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1538,16 +1606,16 @@
         <v>27</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J19" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1570,21 +1638,21 @@
         <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J20" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -1602,16 +1670,19 @@
         <v>27</v>
       </c>
       <c r="H21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>143</v>
+      </c>
+      <c r="M21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>6</v>
       </c>
@@ -1634,16 +1705,19 @@
         <v>27</v>
       </c>
       <c r="H22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I22" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J22" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>145</v>
+      </c>
+      <c r="K22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1666,16 +1740,16 @@
         <v>27</v>
       </c>
       <c r="H23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1698,21 +1772,21 @@
         <v>27</v>
       </c>
       <c r="H24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J24" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -1730,144 +1804,144 @@
         <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I25" t="s">
+        <v>103</v>
+      </c>
+      <c r="J25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="1" customFormat="1">
+      <c r="A26" s="1">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+      <c r="E26" s="1">
+        <v>6136</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J25" t="s">
+    </row>
+    <row r="27" spans="1:13" s="1" customFormat="1">
+      <c r="A27" s="1">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3717</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="1" customFormat="1">
+      <c r="A28" s="1">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>9</v>
+      </c>
+      <c r="E28" s="1">
+        <v>140</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="1" customFormat="1">
+      <c r="A29" s="1">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1">
+        <v>35</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>4</v>
-      </c>
-      <c r="E26">
-        <v>6136</v>
-      </c>
-      <c r="F26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" t="s">
-        <v>75</v>
-      </c>
-      <c r="I26" t="s">
-        <v>106</v>
-      </c>
-      <c r="J26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>4</v>
-      </c>
-      <c r="E27">
-        <v>3717</v>
-      </c>
-      <c r="F27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" t="s">
-        <v>76</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="J29" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="J27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>9</v>
-      </c>
-      <c r="E28">
-        <v>140</v>
-      </c>
-      <c r="F28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" t="s">
-        <v>28</v>
-      </c>
-      <c r="H28" t="s">
-        <v>77</v>
-      </c>
-      <c r="I28" t="s">
-        <v>154</v>
-      </c>
-      <c r="J28" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>8</v>
-      </c>
-      <c r="E29">
-        <v>35</v>
-      </c>
-      <c r="F29" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" t="s">
-        <v>78</v>
-      </c>
-      <c r="I29" t="s">
-        <v>156</v>
-      </c>
-      <c r="J29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30">
         <v>8</v>
       </c>
@@ -1890,16 +1964,16 @@
         <v>23</v>
       </c>
       <c r="H30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I30" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J30" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31">
         <v>8</v>
       </c>
@@ -1922,16 +1996,16 @@
         <v>23</v>
       </c>
       <c r="H31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I31" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J31" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32">
         <v>8</v>
       </c>
@@ -1954,21 +2028,21 @@
         <v>23</v>
       </c>
       <c r="H32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I32" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33">
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>136</v>
+        <v>47</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -1986,21 +2060,27 @@
         <v>23</v>
       </c>
       <c r="H33" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="I33" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+        <v>111</v>
+      </c>
+      <c r="L33" t="s">
+        <v>167</v>
+      </c>
+      <c r="N33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34">
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" t="b">
         <v>1</v>
@@ -2021,13 +2101,13 @@
         <v>51</v>
       </c>
       <c r="I34" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J34" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35">
         <v>9</v>
       </c>
@@ -2050,16 +2130,16 @@
         <v>29</v>
       </c>
       <c r="H35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J35" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36">
         <v>9</v>
       </c>
@@ -2082,21 +2162,24 @@
         <v>29</v>
       </c>
       <c r="H36" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
       <c r="I36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J36" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+        <v>162</v>
+      </c>
+      <c r="L36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37">
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>171</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -2114,13 +2197,86 @@
         <v>29</v>
       </c>
       <c r="H37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J37" t="s">
-        <v>167</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="B40" t="s">
+        <v>173</v>
+      </c>
+      <c r="L40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="B41" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="B42" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="B43" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="B44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="B45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="B46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="B47" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>